<commit_message>
Cambios de organizacion y limpieza
</commit_message>
<xml_diff>
--- a/PRTC_Hotels_Prices_2026-02-03.xlsx
+++ b/PRTC_Hotels_Prices_2026-02-03.xlsx
@@ -955,7 +955,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M153"/>
+  <dimension ref="A1:O153"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="J1" s="3" t="inlineStr">
         <is>
-          <t>Xotelo_Price_USD</t>
+          <t>Price_USD</t>
         </is>
       </c>
       <c r="K1" s="3" t="inlineStr">
@@ -1024,6 +1024,16 @@
       <c r="M1" s="3" t="inlineStr">
         <is>
           <t>Search_Params</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>Date_Found</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>Source</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1081,13 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1139,13 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>xotelo</t>
         </is>
       </c>
     </row>
@@ -1164,7 +1186,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1174,7 +1196,13 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>xotelo</t>
         </is>
       </c>
     </row>
@@ -1225,7 +1253,13 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>xotelo</t>
         </is>
       </c>
     </row>
@@ -1261,9 +1295,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J6" t="n">
+        <v>215</v>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Google Hotels</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1273,7 +1310,13 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>serpapi</t>
         </is>
       </c>
     </row>
@@ -1310,11 +1353,11 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>908</v>
+        <v>1028</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t xml:space="preserve"> Official Site</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1324,7 +1367,13 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1361,11 +1410,11 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1375,7 +1424,13 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1411,9 +1466,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J9" t="n">
+        <v>431</v>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Trip.com</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1423,7 +1481,13 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>xotelo:+60d</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1524,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1474,7 +1538,13 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1525,7 +1595,13 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1652,13 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1613,11 +1695,11 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>411</v>
+        <v>344</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Trip.com</t>
+          <t>Official Hotel</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1627,7 +1709,13 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1678,7 +1766,13 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1714,9 +1808,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J15" t="n">
+        <v>569</v>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1726,7 +1823,13 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>xotelo:+60d</t>
         </is>
       </c>
     </row>
@@ -1763,11 +1866,11 @@
         </is>
       </c>
       <c r="J16" t="n">
-        <v>762</v>
+        <v>662</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Trip.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1777,7 +1880,13 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1814,11 +1923,11 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1828,7 +1937,13 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1994,13 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1916,11 +2037,11 @@
         </is>
       </c>
       <c r="J19" t="n">
-        <v>584</v>
+        <v>531</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Olive Boutique</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1930,7 +2051,13 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -1967,7 +2094,7 @@
         </is>
       </c>
       <c r="J20" t="n">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -1981,7 +2108,13 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2018,7 +2151,7 @@
         </is>
       </c>
       <c r="J21" t="n">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -2032,7 +2165,13 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2083,7 +2222,13 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2134,7 +2279,13 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2185,7 +2336,13 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2236,7 +2393,13 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2450,13 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2335,7 +2504,13 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -2372,11 +2547,11 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2386,7 +2561,13 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2423,7 +2604,7 @@
         </is>
       </c>
       <c r="J29" t="n">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -2437,7 +2618,13 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2488,7 +2675,13 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2539,7 +2732,13 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2590,7 +2789,13 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2627,11 +2832,11 @@
         </is>
       </c>
       <c r="J33" t="n">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2641,7 +2846,13 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2677,9 +2888,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J34" t="n">
+        <v>583</v>
+      </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2689,7 +2903,13 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>xotelo:weekend</t>
         </is>
       </c>
     </row>
@@ -2726,11 +2946,11 @@
         </is>
       </c>
       <c r="J35" t="n">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t xml:space="preserve"> Official Site</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2740,7 +2960,13 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2777,11 +3003,11 @@
         </is>
       </c>
       <c r="J36" t="n">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -2791,7 +3017,13 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2827,9 +3059,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J37" t="n">
+        <v>270</v>
+      </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -2839,7 +3074,13 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>xotelo:+90d</t>
         </is>
       </c>
     </row>
@@ -2876,11 +3117,11 @@
         </is>
       </c>
       <c r="J38" t="n">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -2890,7 +3131,13 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2941,7 +3188,13 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -2972,6 +3225,28 @@
       <c r="F40" t="n">
         <v>202512</v>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3017,7 +3292,13 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -3054,11 +3335,11 @@
         </is>
       </c>
       <c r="J42" t="n">
-        <v>263</v>
+        <v>317</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Trip.com</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3068,7 +3349,13 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3105,11 +3392,11 @@
         </is>
       </c>
       <c r="J43" t="n">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Official Site</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3119,7 +3406,13 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3170,7 +3463,13 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3206,9 +3505,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J45" t="n">
+        <v>202</v>
+      </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3218,7 +3520,13 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>xotelo:+90d</t>
         </is>
       </c>
     </row>
@@ -3255,11 +3563,11 @@
         </is>
       </c>
       <c r="J46" t="n">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Official Site</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3269,7 +3577,13 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3305,9 +3619,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J47" t="n">
+        <v>322</v>
+      </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3317,7 +3634,13 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>xotelo:weekend</t>
         </is>
       </c>
     </row>
@@ -3368,7 +3691,13 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3405,7 +3734,7 @@
         </is>
       </c>
       <c r="J49" t="n">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -3419,7 +3748,13 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3470,7 +3805,13 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3521,7 +3862,13 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3572,7 +3919,13 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3623,7 +3976,13 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3660,11 +4019,11 @@
         </is>
       </c>
       <c r="J54" t="n">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Official Site</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -3674,7 +4033,13 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3725,7 +4090,13 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -3761,9 +4132,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J56" t="n">
+        <v>569</v>
+      </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -3773,7 +4147,13 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>xotelo:+60d</t>
         </is>
       </c>
     </row>
@@ -3821,7 +4201,13 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -3857,9 +4243,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J58" t="n">
+        <v>134</v>
+      </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
@@ -3869,7 +4258,13 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>xotelo:+90d</t>
         </is>
       </c>
     </row>
@@ -3905,9 +4300,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J59" t="n">
+        <v>148.65</v>
+      </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
@@ -3917,7 +4315,13 @@
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>apify</t>
         </is>
       </c>
     </row>
@@ -3968,7 +4372,13 @@
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4005,11 +4415,11 @@
         </is>
       </c>
       <c r="J61" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -4019,7 +4429,13 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4070,7 +4486,13 @@
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4107,7 +4529,7 @@
         </is>
       </c>
       <c r="J63" t="n">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
@@ -4121,7 +4543,13 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4158,7 +4586,7 @@
         </is>
       </c>
       <c r="J64" t="n">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -4172,7 +4600,13 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4223,7 +4657,13 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4274,7 +4714,13 @@
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4310,9 +4756,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J67" t="n">
+        <v>262</v>
+      </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Google Hotels</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -4322,7 +4771,13 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>serpapi</t>
         </is>
       </c>
     </row>
@@ -4370,7 +4825,13 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -4421,7 +4882,13 @@
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4457,9 +4924,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J70" t="n">
+        <v>165</v>
+      </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -4469,7 +4939,13 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>xotelo:+90d</t>
         </is>
       </c>
     </row>
@@ -4520,7 +4996,13 @@
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4557,7 +5039,7 @@
         </is>
       </c>
       <c r="J72" t="n">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -4571,7 +5053,13 @@
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4622,7 +5110,13 @@
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4673,7 +5167,13 @@
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4724,7 +5224,13 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4760,9 +5266,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J76" t="n">
+        <v>194</v>
+      </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Trip.com</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -4772,7 +5281,13 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>xotelo:+90d</t>
         </is>
       </c>
     </row>
@@ -4823,7 +5338,13 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4860,11 +5381,11 @@
         </is>
       </c>
       <c r="J78" t="n">
-        <v>255</v>
+        <v>180</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
@@ -4874,7 +5395,13 @@
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4925,7 +5452,13 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -4976,7 +5509,13 @@
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5027,7 +5566,13 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5063,9 +5608,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J82" t="n">
+        <v>100</v>
+      </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -5075,7 +5623,13 @@
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>apify</t>
         </is>
       </c>
     </row>
@@ -5126,7 +5680,13 @@
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5174,7 +5734,13 @@
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -5210,9 +5776,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J85" t="n">
+        <v>135</v>
+      </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -5222,7 +5791,13 @@
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5259,11 +5834,11 @@
         </is>
       </c>
       <c r="J86" t="n">
-        <v>305</v>
+        <v>258</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -5273,7 +5848,13 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5309,9 +5890,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J87" t="n">
+        <v>216</v>
+      </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
@@ -5321,7 +5905,13 @@
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5358,11 +5948,11 @@
         </is>
       </c>
       <c r="J88" t="n">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Trip.com</t>
         </is>
       </c>
       <c r="L88" t="inlineStr">
@@ -5372,7 +5962,13 @@
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5420,7 +6016,13 @@
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -5471,7 +6073,13 @@
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5507,9 +6115,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J91" t="n">
+        <v>139</v>
+      </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L91" t="inlineStr">
@@ -5519,7 +6130,13 @@
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5555,9 +6172,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J92" t="n">
+        <v>130.37</v>
+      </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L92" t="inlineStr">
@@ -5567,7 +6187,13 @@
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>apify</t>
         </is>
       </c>
     </row>
@@ -5618,7 +6244,13 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5655,7 +6287,7 @@
         </is>
       </c>
       <c r="J94" t="n">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
@@ -5669,7 +6301,13 @@
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5706,11 +6344,11 @@
         </is>
       </c>
       <c r="J95" t="n">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L95" t="inlineStr">
@@ -5720,7 +6358,13 @@
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5756,9 +6400,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J96" t="n">
+        <v>583</v>
+      </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L96" t="inlineStr">
@@ -5768,7 +6415,13 @@
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>xotelo:weekend</t>
         </is>
       </c>
     </row>
@@ -5799,6 +6452,28 @@
       <c r="F97" t="n">
         <v>202512</v>
       </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5847,7 +6522,13 @@
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5898,7 +6579,13 @@
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5935,11 +6622,11 @@
         </is>
       </c>
       <c r="J100" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L100" t="inlineStr">
@@ -5949,7 +6636,13 @@
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -5986,11 +6679,11 @@
         </is>
       </c>
       <c r="J101" t="n">
-        <v>232</v>
+        <v>134</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L101" t="inlineStr">
@@ -6000,7 +6693,13 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6037,11 +6736,11 @@
         </is>
       </c>
       <c r="J102" t="n">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L102" t="inlineStr">
@@ -6051,7 +6750,13 @@
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6088,11 +6793,11 @@
         </is>
       </c>
       <c r="J103" t="n">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L103" t="inlineStr">
@@ -6102,7 +6807,13 @@
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6153,7 +6864,13 @@
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6190,7 +6907,7 @@
         </is>
       </c>
       <c r="J105" t="n">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -6204,7 +6921,13 @@
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6252,7 +6975,13 @@
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -6300,7 +7029,13 @@
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -6336,9 +7071,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J108" t="n">
+        <v>122</v>
+      </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L108" t="inlineStr">
@@ -6348,7 +7086,13 @@
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>xotelo:+90d</t>
         </is>
       </c>
     </row>
@@ -6399,7 +7143,13 @@
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6435,9 +7185,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J110" t="n">
+        <v>302</v>
+      </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Google Hotels</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
@@ -6447,7 +7200,13 @@
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>serpapi</t>
         </is>
       </c>
     </row>
@@ -6495,7 +7254,13 @@
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -6546,7 +7311,13 @@
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6594,7 +7365,13 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -6645,7 +7422,13 @@
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6693,7 +7476,13 @@
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -6741,7 +7530,13 @@
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -6792,7 +7587,13 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6840,7 +7641,13 @@
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr"/>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -6876,9 +7683,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J119" t="n">
+        <v>362.6</v>
+      </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L119" t="inlineStr">
@@ -6888,7 +7698,13 @@
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr"/>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>apify</t>
         </is>
       </c>
     </row>
@@ -6939,7 +7755,13 @@
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr"/>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -6987,7 +7809,13 @@
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr"/>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -7038,7 +7866,13 @@
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7086,7 +7920,13 @@
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -7122,9 +7962,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J124" t="n">
+        <v>104</v>
+      </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="L124" t="inlineStr">
@@ -7134,7 +7977,13 @@
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>xotelo:+60d</t>
         </is>
       </c>
     </row>
@@ -7182,7 +8031,13 @@
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr"/>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -7233,7 +8088,13 @@
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N126" t="inlineStr"/>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7270,11 +8131,11 @@
         </is>
       </c>
       <c r="J127" t="n">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="K127" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L127" t="inlineStr">
@@ -7284,7 +8145,13 @@
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr"/>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7335,7 +8202,13 @@
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr"/>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7386,7 +8259,13 @@
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N129" t="inlineStr"/>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7437,7 +8316,13 @@
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7474,11 +8359,11 @@
         </is>
       </c>
       <c r="J131" t="n">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L131" t="inlineStr">
@@ -7488,7 +8373,13 @@
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7536,7 +8427,13 @@
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N132" t="inlineStr"/>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -7573,11 +8470,11 @@
         </is>
       </c>
       <c r="J133" t="n">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L133" t="inlineStr">
@@ -7587,7 +8484,13 @@
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N133" t="inlineStr"/>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7635,7 +8538,13 @@
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N134" t="inlineStr"/>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -7686,7 +8595,13 @@
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N135" t="inlineStr"/>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7723,11 +8638,11 @@
         </is>
       </c>
       <c r="J136" t="n">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L136" t="inlineStr">
@@ -7737,7 +8652,13 @@
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7774,11 +8695,11 @@
         </is>
       </c>
       <c r="J137" t="n">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="L137" t="inlineStr">
@@ -7788,7 +8709,13 @@
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N137" t="inlineStr"/>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7825,7 +8752,7 @@
         </is>
       </c>
       <c r="J138" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K138" t="inlineStr">
         <is>
@@ -7839,7 +8766,13 @@
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N138" t="inlineStr"/>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7876,7 +8809,7 @@
         </is>
       </c>
       <c r="J139" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K139" t="inlineStr">
         <is>
@@ -7890,7 +8823,13 @@
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N139" t="inlineStr"/>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -7938,7 +8877,13 @@
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N140" t="inlineStr"/>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -7986,7 +8931,13 @@
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N141" t="inlineStr"/>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -8023,11 +8974,11 @@
         </is>
       </c>
       <c r="J142" t="n">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="K142" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L142" t="inlineStr">
@@ -8037,7 +8988,13 @@
       </c>
       <c r="M142" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N142" t="inlineStr"/>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -8073,9 +9030,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J143" t="n">
+        <v>133</v>
+      </c>
       <c r="K143" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="L143" t="inlineStr">
@@ -8085,7 +9045,13 @@
       </c>
       <c r="M143" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N143" t="inlineStr"/>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>xotelo:+90d</t>
         </is>
       </c>
     </row>
@@ -8133,7 +9099,13 @@
       </c>
       <c r="M144" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr"/>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -8181,7 +9153,13 @@
       </c>
       <c r="M145" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -8212,6 +9190,31 @@
       <c r="F146" t="n">
         <v>202512</v>
       </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="J146" t="n">
+        <v>145</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>Google Hotels</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N146" t="inlineStr"/>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>serpapi</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -8260,7 +9263,13 @@
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N147" t="inlineStr"/>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>
@@ -8308,7 +9317,13 @@
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N148" t="inlineStr"/>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -8356,7 +9371,13 @@
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N149" t="inlineStr"/>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -8404,7 +9425,13 @@
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr"/>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
@@ -8440,9 +9467,12 @@
           <t>2026-02-03</t>
         </is>
       </c>
+      <c r="J151" t="n">
+        <v>106</v>
+      </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Official Hotel Site</t>
         </is>
       </c>
       <c r="L151" t="inlineStr">
@@ -8452,7 +9482,13 @@
       </c>
       <c r="M151" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>xotelo:+60d</t>
         </is>
       </c>
     </row>
@@ -8503,7 +9539,13 @@
       </c>
       <c r="M152" t="inlineStr">
         <is>
-          <t>2026-03-05 to 2026-03-06 | 1rm/2ad</t>
+          <t>2026-03-05 to 2026-03-06 | 1rm/2ad (multi-date) (cascade)</t>
+        </is>
+      </c>
+      <c r="N152" t="inlineStr"/>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>xotelo:+30d</t>
         </is>
       </c>
     </row>

</xml_diff>